<commit_message>
Ready for first release
</commit_message>
<xml_diff>
--- a/portfolio-matrices/portfolio-matrix-temp.xlsx
+++ b/portfolio-matrices/portfolio-matrix-temp.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,42 +468,1062 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>41274</v>
+        <v>43465</v>
       </c>
       <c r="B2" t="n">
-        <v>0.1837658832215003</v>
+        <v>0.1674260248852195</v>
       </c>
       <c r="C2" t="n">
-        <v>0.2025518932256514</v>
+        <v>0.1930020894201169</v>
       </c>
       <c r="D2" t="n">
-        <v>0.1938869847975864</v>
+        <v>0.2008584784169489</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2317774715223708</v>
+        <v>0.2521859475325305</v>
       </c>
       <c r="F2" t="n">
-        <v>0.1880177672328911</v>
+        <v>0.1865274597451842</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>43098</v>
+        <v>43472</v>
       </c>
       <c r="B3" t="n">
-        <v>0.1680455608320196</v>
+        <v>0.166588860797191</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2030826168865876</v>
+        <v>0.1959677722116826</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1971195806835036</v>
+        <v>0.2002349886420789</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2510710160331098</v>
+        <v>0.2527817314512487</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1806812255647795</v>
+        <v>0.1844266468977989</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="n">
+        <v>43479</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1663402133988945</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.1964513693758249</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.2000530479034247</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.2529349915122709</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.1842203778095849</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="n">
+        <v>43486</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.1657633788830777</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.1976387396537541</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.2000386730908858</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.2534967928255785</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.1830624155467038</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="n">
+        <v>43493</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.1662274728382129</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.1967288498629748</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.1996347487142792</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.2537667705899903</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.1836421579945428</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="n">
+        <v>43500</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.166452236880124</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.1973265279880034</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.1987844402222383</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.252717746165192</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.1847190487444424</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="n">
+        <v>43507</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.1667843177999979</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.1974781915148041</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.1989572428316627</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.2514529016960957</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.1853273461574398</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="n">
+        <v>43514</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.165777693928016</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1988219347481669</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.1980171828735866</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.2525897961272004</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.18479339232303</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>43521</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.1658066152508513</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.198064806424449</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.1976585935530206</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.2535984232595164</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.1848715615121626</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="n">
+        <v>43528</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.1652748626630469</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.1977661799791609</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.1974150506626761</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.2548614550809505</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.1846824516141655</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="n">
+        <v>43535</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.1657231958098631</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.1970557716875933</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.1979944464977778</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.2539489107340679</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.1852776752706977</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="n">
+        <v>43542</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.1651956901552518</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.1989139859326077</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.1972848662127087</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.2538728957625609</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.1847325619368707</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="n">
+        <v>43549</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.165469038015123</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.1970853562680343</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.1989650205553242</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.2529760793696832</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.1855045057918354</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="n">
+        <v>43556</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.1652936583837338</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.1981172258807877</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.1982032712594858</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.2528341032298894</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.1855517412461033</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
+        <v>43563</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.1652090345154937</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.1987626397162592</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.1980561796657293</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.2524744474915687</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.1854976986109489</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>43570</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.1650804425589615</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.1988394886098266</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.197933696241865</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.2528690654135198</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.1852773071758272</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>43577</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.1651082194878623</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.199293805834217</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.1973029349885051</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.2533700659125685</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.1849249737768471</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>43584</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.1652747478045473</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.1988916112524657</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.1973742363606403</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.253358756798767</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.1851006477835797</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>43591</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.1653391019966403</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.1981522162227579</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0.1979290137057216</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.2531310310433805</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.1854486370314998</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="n">
+        <v>43598</v>
+      </c>
+      <c r="B21" t="n">
+        <v>0.1656667607318793</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0.1971408053501334</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.1987084390023025</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0.2528441612782902</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0.1856398336373947</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>43605</v>
+      </c>
+      <c r="B22" t="n">
+        <v>0.1656524503555094</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0.1974805554287444</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.1984516541478849</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0.2529712418838471</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.1854440981840141</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="n">
+        <v>43612</v>
+      </c>
+      <c r="B23" t="n">
+        <v>0.1656333323953316</v>
+      </c>
+      <c r="C23" t="n">
+        <v>0.1973733587644843</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.1984801753172483</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.2531354370310606</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.1853776964918752</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="n">
+        <v>43619</v>
+      </c>
+      <c r="B24" t="n">
+        <v>0.1657930925607262</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.1970301733078422</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.1987596660967099</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0.2526602784971786</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.1857567895375429</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="n">
+        <v>43626</v>
+      </c>
+      <c r="B25" t="n">
+        <v>0.1656627074230863</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.1978291371461668</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.1984136303149413</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0.2529197019662797</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.1851748231495258</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="n">
+        <v>43633</v>
+      </c>
+      <c r="B26" t="n">
+        <v>0.1653938724669232</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.1977524790800575</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.1983662916849248</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.2529094211844621</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.1855779355836324</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="n">
+        <v>43640</v>
+      </c>
+      <c r="B27" t="n">
+        <v>0.1650971859258622</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.1981756711021548</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.1978327670757472</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0.2533266118628488</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.185567764033387</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="n">
+        <v>43647</v>
+      </c>
+      <c r="B28" t="n">
+        <v>0.1654832665226579</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.1983466078752031</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.1977347837129832</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0.2526982542797438</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.1857370876094122</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="n">
+        <v>43654</v>
+      </c>
+      <c r="B29" t="n">
+        <v>0.1649227274434195</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0.1983379598409707</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0.1979308546579211</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0.2528273204290268</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.1859811376286619</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="n">
+        <v>43661</v>
+      </c>
+      <c r="B30" t="n">
+        <v>0.1661440054162444</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.1979744700114354</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.1978351507166425</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0.2525848864728885</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.1854614873827894</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="n">
+        <v>43668</v>
+      </c>
+      <c r="B31" t="n">
+        <v>0.1667275572001527</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.1975430695814343</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.1977830716337305</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0.2520661381608664</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.185880163423816</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="n">
+        <v>43675</v>
+      </c>
+      <c r="B32" t="n">
+        <v>0.1670824408090954</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.1979829123825437</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.1980256922336531</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.2508153720118536</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.1860935825628542</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="n">
+        <v>43682</v>
+      </c>
+      <c r="B33" t="n">
+        <v>0.1675606282287573</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.1956546664657439</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.1984580373211278</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0.2521812667016459</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.186145401282725</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="n">
+        <v>43689</v>
+      </c>
+      <c r="B34" t="n">
+        <v>0.1674118747335636</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.195760466687388</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.1984713499858383</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0.2521391294223389</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.1862171791708712</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="n">
+        <v>43696</v>
+      </c>
+      <c r="B35" t="n">
+        <v>0.1684041541562922</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.1948537640498632</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.1990853253533387</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0.2503545751094676</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.1873021813310383</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="n">
+        <v>43703</v>
+      </c>
+      <c r="B36" t="n">
+        <v>0.1687393196712539</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.1950054371889405</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.1993477000732411</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0.2494301978726526</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.187477345193912</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="n">
+        <v>43710</v>
+      </c>
+      <c r="B37" t="n">
+        <v>0.1686469960750284</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.1948199633293682</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.1990331452963791</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.2501982585857572</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.1873016367134671</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="n">
+        <v>43717</v>
+      </c>
+      <c r="B38" t="n">
+        <v>0.1683759994868926</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.1951645926575123</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.1988473651098021</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0.2506049476289728</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.1870070951168201</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="n">
+        <v>43724</v>
+      </c>
+      <c r="B39" t="n">
+        <v>0.1684558014027256</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.1952496972850521</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.1987973087966202</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0.2507470179929339</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.1867501745226684</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="n">
+        <v>43731</v>
+      </c>
+      <c r="B40" t="n">
+        <v>0.1685323794151093</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.1950857696050245</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.1989320033684923</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0.2506242380361466</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.1868256095752273</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="n">
+        <v>43738</v>
+      </c>
+      <c r="B41" t="n">
+        <v>0.1685666580422436</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.1952175094459173</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0.1989792817760071</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0.2504124854577224</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.1868240652781097</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="n">
+        <v>43745</v>
+      </c>
+      <c r="B42" t="n">
+        <v>0.1688421775918365</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.1952689659530843</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.1990444202279207</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0.2495046734260613</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.1873397628010972</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>43752</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.1686448806914828</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.1951904599594261</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.1988272905345033</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0.250366439999513</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.1869709288150746</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>43759</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.1686751375408838</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.1949044960317774</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.1989417225259295</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0.2505783755135622</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.1869002683878472</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>43766</v>
+      </c>
+      <c r="B45" t="n">
+        <v>0.1686652694325857</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.194659492184606</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.1989708535766916</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.2506628591982095</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.1870415256079073</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>43773</v>
+      </c>
+      <c r="B46" t="n">
+        <v>0.1685022635190223</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.1940989262342342</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0.1990495435568801</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.2499034347222945</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.1884458319675687</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="n">
+        <v>43780</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.168851602964315</v>
+      </c>
+      <c r="C47" t="n">
+        <v>0.1941670043430785</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.1990094692333766</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.249288900652882</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.188683022806348</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>43787</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0.1690762361123915</v>
+      </c>
+      <c r="C48" t="n">
+        <v>0.1944838495705498</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.1989244570933907</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.2488730221504392</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.1886424350732289</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>43794</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0.1691191464521638</v>
+      </c>
+      <c r="C49" t="n">
+        <v>0.1949553397246663</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.1987234989438077</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.2486540084236691</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.188548006455693</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>43801</v>
+      </c>
+      <c r="B50" t="n">
+        <v>0.1689980296166013</v>
+      </c>
+      <c r="C50" t="n">
+        <v>0.1964904216286529</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.1986235761651818</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.2476827073519936</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.1882052652375704</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>43808</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0.1689256992537485</v>
+      </c>
+      <c r="C51" t="n">
+        <v>0.1961927678957719</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.198492340436957</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.2485579622704055</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.1878312301431171</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>43815</v>
+      </c>
+      <c r="B52" t="n">
+        <v>0.169425267208353</v>
+      </c>
+      <c r="C52" t="n">
+        <v>0.1957020640482689</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.1986430984705207</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.2481262810442869</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.1881032892285706</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>43822</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0.1690582537373573</v>
+      </c>
+      <c r="C53" t="n">
+        <v>0.1968150200872298</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.1985654903877383</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.2474140645647323</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.1881471712229423</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="n">
+        <v>43829</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0.1691865211699197</v>
+      </c>
+      <c r="C54" t="n">
+        <v>0.195539280183792</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.19897968052891</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0.2478481647617837</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.1884463533555947</v>
       </c>
     </row>
   </sheetData>

</xml_diff>